<commit_message>
Created benchmark statisctics for 1988-2000 range
</commit_message>
<xml_diff>
--- a/SEER analysis/OverallSurvivalBySex2004+.xlsx
+++ b/SEER analysis/OverallSurvivalBySex2004+.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janek/Documents/GitHub/CMOSTv2/SEER analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpoleszczuk\Documents\GitHub\CMOSTv2\SEER analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D46EF7C7-6988-7646-BF71-CCB8014D2AC3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22860" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22860" windowHeight="16065"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -55,7 +54,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -388,6 +387,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -413,7 +413,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -451,7 +451,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1949116863"/>
@@ -508,6 +508,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -533,7 +534,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="pl-PL"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -565,7 +566,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="pl-PL"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1949198095"/>
@@ -582,6 +583,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -607,12 +609,13 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="pl-PL"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -620,7 +623,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -644,7 +646,7 @@
       <a:pPr>
         <a:defRPr sz="1400"/>
       </a:pPr>
-      <a:endParaRPr lang="pl-PL"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1530,19 +1532,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R37" sqref="R37"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1568,7 +1570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1594,7 +1596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>0.82207631887494304</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>0.73115373404512396</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1672,7 +1674,7 @@
         <v>0.660757579839926</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1698,7 +1700,7 @@
         <v>0.60685355491096804</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1724,7 +1726,7 @@
         <v>0.56412712326634995</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1750,7 +1752,7 @@
         <v>0.52809551949423195</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1776,7 +1778,7 @@
         <v>0.49678284397536299</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1802,7 +1804,7 @@
         <v>0.46950453506984302</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -1828,7 +1830,7 @@
         <v>0.44545739868789203</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1854,7 +1856,7 @@
         <v>0.423003925249194</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1880,7 +1882,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1906,7 +1908,7 @@
         <v>0.80486515515864399</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -1932,7 +1934,7 @@
         <v>0.717186541435753</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1958,7 +1960,7 @@
         <v>0.65355828010122197</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v>0.60549088534196804</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -2010,7 +2012,7 @@
         <v>0.56555485904226499</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -2036,7 +2038,7 @@
         <v>0.532757172439011</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -2062,7 +2064,7 @@
         <v>0.50363615304444398</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2088,7 +2090,7 @@
         <v>0.47742039604713499</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -2114,7 +2116,7 @@
         <v>0.45437940225769402</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>8</v>
       </c>

</xml_diff>